<commit_message>
update matrix and calculations
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14900"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13780"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="33">
   <si>
     <t>Morphine</t>
   </si>
@@ -111,17 +111,20 @@
     <t>check_amr_low</t>
   </si>
   <si>
-    <t>c,d</t>
-  </si>
-  <si>
-    <t>5,6,7,8,9,10,11,c,d</t>
+    <t>6,7,8,9,10,11,a,b,c,d</t>
+  </si>
+  <si>
+    <t>a,b,c,d</t>
+  </si>
+  <si>
+    <t>8,9,10,11,a,b,c,d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +267,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -566,7 +585,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -609,6 +628,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -620,7 +645,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="48">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -649,11 +674,17 @@
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="28" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="29" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="30" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="31" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="32" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="33" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="34" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="35" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="36" builtinId="28" customBuiltin="1"/>
@@ -957,17 +988,21 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" bestFit="1" customWidth="1"/>
@@ -1019,20 +1054,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2"/>
       <c r="L2"/>
@@ -1048,20 +1083,20 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="2"/>
       <c r="L3"/>
@@ -1077,20 +1112,20 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="2"/>
       <c r="L4"/>
@@ -1106,20 +1141,20 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="2"/>
       <c r="L5"/>
@@ -1135,20 +1170,20 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="2"/>
       <c r="L6"/>
@@ -1164,20 +1199,20 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" s="2"/>
       <c r="L7"/>
@@ -1193,20 +1228,20 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" s="2"/>
       <c r="L8"/>
@@ -1222,20 +1257,20 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="2"/>
       <c r="L9"/>
@@ -1251,20 +1286,20 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="2"/>
       <c r="L10"/>
@@ -1280,20 +1315,20 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="2"/>
       <c r="L11"/>
@@ -1309,20 +1344,20 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="2"/>
       <c r="L12"/>
@@ -1338,20 +1373,20 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="2"/>
       <c r="L13"/>
@@ -1367,20 +1402,20 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="2"/>
       <c r="L14"/>
@@ -1396,20 +1431,20 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="2"/>
       <c r="L15"/>
@@ -1426,19 +1461,19 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J16" s="2"/>
       <c r="L16"/>
@@ -1455,19 +1490,19 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J17" s="2"/>
       <c r="L17"/>
@@ -1484,20 +1519,20 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L18"/>
     </row>
@@ -1513,19 +1548,19 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J19" s="2"/>
       <c r="L19"/>
@@ -1542,20 +1577,20 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L20"/>
     </row>
@@ -1571,22 +1606,20 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="L21"/>
     </row>

</xml_diff>

<commit_message>
update qa and matrix config files
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20560" windowHeight="12160"/>
   </bookViews>
   <sheets>
-    <sheet name="QA" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="QA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -104,9 +108,6 @@
     <t>Hydromorphone-3-B-D-glucuronide</t>
   </si>
   <si>
-    <t>a,b,c,d</t>
-  </si>
-  <si>
     <t>Oxymorphone Glucuronide</t>
   </si>
   <si>
@@ -114,39 +115,22 @@
   </si>
   <si>
     <t>Norbuprenorphine glucuronide</t>
+  </si>
+  <si>
+    <t>b,d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0" numFmtId="165"/>
-    <numFmt formatCode="H:MM" numFmtId="166"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +142,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -166,119 +150,378 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100">
-      <pane activePane="topLeft" topLeftCell="A1" xSplit="0" ySplit="-1"/>
-      <selection activeCell="G21" activeCellId="0" pane="topLeft" sqref="G21"/>
-      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.0313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="17.0862745098039"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8823529411765"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.9019607843137"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="2">
-      <c r="A2" s="0" t="s">
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -299,14 +542,14 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="3">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -327,14 +570,14 @@
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -355,14 +598,14 @@
       </c>
       <c r="J4" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -383,14 +626,14 @@
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -411,14 +654,14 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -439,14 +682,14 @@
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -467,14 +710,14 @@
       </c>
       <c r="J8" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -495,14 +738,14 @@
       </c>
       <c r="J9" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -523,14 +766,14 @@
       </c>
       <c r="J10" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="11">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -551,14 +794,14 @@
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="12">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="n">
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
@@ -579,14 +822,14 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.6" outlineLevel="0" r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -607,14 +850,14 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="14">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -635,14 +878,14 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -663,14 +906,14 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="16">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="3"/>
@@ -691,14 +934,14 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="17">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="3"/>
@@ -719,14 +962,14 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="18">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18" s="3"/>
@@ -744,17 +987,17 @@
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="19">
-      <c r="A19" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="3"/>
@@ -775,14 +1018,14 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="20">
-      <c r="A20" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="2" t="n">
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="3"/>
@@ -800,17 +1043,17 @@
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.25" outlineLevel="0" r="21">
-      <c r="A21" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="2" t="n">
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="3"/>
@@ -828,16 +1071,16 @@
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tests for calculations, fixed typo in matrix.csv
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -42,9 +42,6 @@
     <t>check_signoise</t>
   </si>
   <si>
-    <t>check_ion_rato</t>
-  </si>
-  <si>
     <t>check_is_peak_area</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>b,d</t>
+  </si>
+  <si>
+    <t>check_ion_ratio</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -505,18 +505,18 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -525,26 +525,26 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -553,26 +553,26 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -581,26 +581,26 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -609,26 +609,26 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -637,26 +637,26 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -665,26 +665,26 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -693,26 +693,26 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -721,26 +721,26 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -749,26 +749,26 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -777,26 +777,26 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -805,26 +805,26 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -833,26 +833,26 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -861,26 +861,26 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -889,26 +889,26 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -918,25 +918,25 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -946,25 +946,25 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -974,25 +974,25 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -1002,25 +1002,25 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -1030,25 +1030,25 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -1058,20 +1058,20 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update matrix and qa files per Jane
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20565" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20560" windowHeight="12160"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="36">
   <si>
     <t>compound_name</t>
   </si>
@@ -120,20 +120,39 @@
     <t>check_ion_ratio</t>
   </si>
   <si>
-    <t>6,7,10,11,b,d</t>
-  </si>
-  <si>
-    <t>8,10,11,b,d</t>
+    <t>check_ion_ratio_std</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5</t>
+  </si>
+  <si>
+    <t>8,10,11,a,c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -156,8 +175,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -169,7 +194,13 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,26 +500,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,13 +546,16 @@
         <v>32</v>
       </c>
       <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -531,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
@@ -544,11 +579,14 @@
         <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -559,7 +597,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
@@ -572,11 +610,14 @@
         <v>10</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -587,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
@@ -600,11 +641,14 @@
         <v>10</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -615,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
@@ -628,11 +672,14 @@
         <v>10</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -643,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
@@ -656,11 +703,14 @@
         <v>10</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -671,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
@@ -684,11 +734,14 @@
         <v>10</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -699,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
@@ -712,11 +765,14 @@
         <v>10</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -727,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
@@ -740,11 +796,14 @@
         <v>10</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -755,7 +814,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
@@ -768,11 +827,14 @@
         <v>10</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -783,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
@@ -796,11 +858,14 @@
         <v>10</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -811,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
@@ -824,11 +889,14 @@
         <v>10</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -839,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
@@ -852,11 +920,14 @@
         <v>10</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -867,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
@@ -880,11 +951,14 @@
         <v>10</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -895,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
@@ -908,11 +982,14 @@
         <v>10</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -924,7 +1001,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>25</v>
@@ -935,12 +1012,13 @@
       <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -952,7 +1030,7 @@
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>25</v>
@@ -963,12 +1041,13 @@
       <c r="H17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -980,7 +1059,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>25</v>
@@ -992,11 +1071,12 @@
         <v>25</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1008,7 +1088,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>25</v>
@@ -1019,12 +1099,13 @@
       <c r="H19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1036,7 +1117,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>25</v>
@@ -1048,11 +1129,12 @@
         <v>25</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1064,7 +1146,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>25</v>
@@ -1076,13 +1158,14 @@
         <v>25</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
updated xls versions of config files - these may not have changed since last update since exported csvs appear identical to last commit
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20560" windowHeight="12160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14840"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
updated matrix file which no longer defined check_amr and check_amr_low; removed these calculations, test pass
</commit_message>
<xml_diff>
--- a/opiate/data/matrix.xlsx
+++ b/opiate/data/matrix.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="33">
   <si>
     <t>compound_name</t>
   </si>
@@ -30,12 +30,6 @@
     <t>check_stda_signoise</t>
   </si>
   <si>
-    <t>check_amr</t>
-  </si>
-  <si>
-    <t>check_amr_low</t>
-  </si>
-  <si>
     <t>check_rrt</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
   </si>
   <si>
     <t>1,2,3,4,5</t>
-  </si>
-  <si>
-    <t>8,10,11,a,c</t>
   </si>
 </sst>
 </file>
@@ -500,27 +491,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,58 +527,48 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>11</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -597,29 +577,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>12</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -628,29 +604,25 @@
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -659,29 +631,25 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -690,29 +658,25 @@
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -721,29 +685,25 @@
         <v>1</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -752,29 +712,25 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -783,29 +739,25 @@
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -814,29 +766,25 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -845,29 +793,25 @@
         <v>1</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -876,29 +820,25 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -907,29 +847,25 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -938,29 +874,25 @@
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -969,29 +901,25 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F15" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11">
+        <v>8</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -999,28 +927,24 @@
       <c r="C16" s="2">
         <v>1</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11">
+        <v>23</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -1028,28 +952,24 @@
       <c r="C17" s="2">
         <v>1</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>25</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" t="s">
-        <v>27</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -1057,28 +977,24 @@
       <c r="C18" s="2">
         <v>1</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E18" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+        <v>23</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -1086,28 +1002,24 @@
       <c r="C19" s="2">
         <v>1</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E19" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11">
+        <v>23</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -1115,28 +1027,24 @@
       <c r="C20" s="2">
         <v>1</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E20" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+        <v>23</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -1144,23 +1052,19 @@
       <c r="C21" s="2">
         <v>1</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E21" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>